<commit_message>
update and correct code
test new version of code
</commit_message>
<xml_diff>
--- a/list_price.xlsx
+++ b/list_price.xlsx
@@ -1,16 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3A67A044-AE58-45E0-A8EA-8C88ACD5AFFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DDE460AF-DCDE-7A4F-907F-B451D003B525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -87,7 +82,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -95,7 +90,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -159,9 +154,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -199,9 +194,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -234,9 +229,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -269,9 +281,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -451,13 +480,13 @@
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.8984375" customWidth="1"/>
-    <col min="2" max="2" width="16.296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.8671875" customWidth="1"/>
+    <col min="2" max="2" width="16.27734375" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -465,7 +494,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -473,7 +502,7 @@
         <v>142000</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -481,7 +510,7 @@
         <v>279000</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -489,7 +518,7 @@
         <v>202000</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -497,7 +526,7 @@
         <v>1058000</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -505,7 +534,7 @@
         <v>2540</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -513,7 +542,7 @@
         <v>2420</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -521,7 +550,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -529,7 +558,7 @@
         <v>16400</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -537,7 +566,7 @@
         <v>34200</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -545,7 +574,7 @@
         <v>30700</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -553,7 +582,7 @@
         <v>27100</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
update code import data
get data from user
</commit_message>
<xml_diff>
--- a/list_price.xlsx
+++ b/list_price.xlsx
@@ -1,16 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DDE460AF-DCDE-7A4F-907F-B451D003B525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github_ripository\knauf_analysis\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C86421D5-5DFF-4337-B9FE-A32B7739785A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -19,7 +25,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -82,7 +87,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -90,7 +95,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -154,9 +159,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -194,9 +199,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -229,26 +234,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -281,26 +269,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -476,17 +447,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.8671875" customWidth="1"/>
-    <col min="2" max="2" width="16.27734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.8984375" customWidth="1"/>
+    <col min="2" max="2" width="16.296875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -494,95 +465,95 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>142000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>154000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>279000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>302000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>202000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>219000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>1058000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>960000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>2540</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3050</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="2">
-        <v>2420</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+        <v>2900</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="2">
-        <v>35000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>16400</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+        <v>17800</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="2">
-        <v>34200</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+        <v>37000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="2">
-        <v>30700</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+        <v>33500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="2">
-        <v>27100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+        <v>29400</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>

</xml_diff>